<commit_message>
updating after final blade tip and drivetrain check
</commit_message>
<xml_diff>
--- a/Documentation/drivetrain/Nacelle_Mass_Properties.xlsx
+++ b/Documentation/drivetrain/Nacelle_Mass_Properties.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gbarter/systems/referenceTurbines/15mw/IEA-15-240-RWT/Documentation/drivetrain/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A65E0DC3-E17E-3940-B5AC-7ACC6A9FC591}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20DDD118-F7EF-4844-A58E-8CBCC2A32E88}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15160" yWindow="1200" windowWidth="26200" windowHeight="12500" xr2:uid="{57C9EAB2-945B-824B-84F5-1D45CDA1F674}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19120" xr2:uid="{57C9EAB2-945B-824B-84F5-1D45CDA1F674}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -23,7 +24,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="40">
   <si>
     <t>Name</t>
   </si>
@@ -99,26 +102,69 @@
     <t>Flange</t>
   </si>
   <si>
-    <t>Shaft bearing 1</t>
-  </si>
-  <si>
-    <t>Shaft bearing 2</t>
+    <t>shaft overhang calc</t>
+  </si>
+  <si>
+    <t>hub radius</t>
+  </si>
+  <si>
+    <t>precone angle</t>
+  </si>
+  <si>
+    <t>previous overhang value</t>
+  </si>
+  <si>
+    <t>deg</t>
+  </si>
+  <si>
+    <t>new overhang value</t>
+  </si>
+  <si>
+    <t>shaft</t>
+  </si>
+  <si>
+    <t>ground x</t>
+  </si>
+  <si>
+    <t>TDO Shaft Bearing</t>
+  </si>
+  <si>
+    <t>SRB Shaft Bearing</t>
+  </si>
+  <si>
+    <t>mass</t>
+  </si>
+  <si>
+    <t>density</t>
+  </si>
+  <si>
+    <t>volume</t>
+  </si>
+  <si>
+    <t>rotor</t>
+  </si>
+  <si>
+    <t>stator</t>
+  </si>
+  <si>
+    <t>Nacelle total minus hub</t>
   </si>
   <si>
     <t>Units</t>
   </si>
   <si>
-    <t>kg</t>
+    <t>t</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.000E+00"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -151,6 +197,20 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -203,7 +263,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -215,27 +275,18 @@
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -550,23 +601,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DE0E285-EA07-5844-9AA6-36952C4B167F}">
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -603,7 +654,7 @@
     </row>
     <row r="2" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>15</v>
@@ -612,7 +663,7 @@
         <v>15</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="E2" s="7" t="s">
         <v>16</v>
@@ -644,30 +695,30 @@
         <f>-0.19</f>
         <v>-0.19</v>
       </c>
-      <c r="D3" s="15">
-        <v>100000</v>
-      </c>
-      <c r="E3" s="11">
+      <c r="D3" s="8">
+        <v>100</v>
+      </c>
+      <c r="E3" s="15">
         <f>490265.833</f>
         <v>490265.83299999998</v>
       </c>
-      <c r="F3" s="11">
+      <c r="F3" s="15">
         <f xml:space="preserve"> 490265.833</f>
         <v>490265.83299999998</v>
       </c>
-      <c r="G3" s="11">
+      <c r="G3" s="15">
         <f xml:space="preserve">  978125</f>
         <v>978125</v>
       </c>
-      <c r="H3" s="11">
+      <c r="H3" s="15">
         <f xml:space="preserve"> 495596.28</f>
         <v>495596.28</v>
       </c>
-      <c r="I3" s="11">
+      <c r="I3" s="15">
         <f>510794.46</f>
         <v>510794.46</v>
       </c>
-      <c r="J3" s="11">
+      <c r="J3" s="15">
         <f>952265.927</f>
         <v>952265.92700000003</v>
       </c>
@@ -676,112 +727,101 @@
       <c r="A4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="8">
-        <v>-6.0750000000000002</v>
-      </c>
-      <c r="C4" s="8">
-        <v>4.9859999999999998</v>
-      </c>
-      <c r="D4" s="15">
-        <v>13362.348</v>
-      </c>
-      <c r="E4" s="11">
-        <f>14765.724</f>
-        <v>14765.724</v>
-      </c>
-      <c r="F4" s="11">
-        <f>14795.619</f>
-        <v>14795.619000000001</v>
-      </c>
-      <c r="G4" s="11">
-        <f>14795.289</f>
-        <v>14795.289000000001</v>
-      </c>
-      <c r="H4" s="11">
-        <f>14765.394</f>
-        <v>14765.394</v>
-      </c>
-      <c r="I4" s="11">
-        <f xml:space="preserve"> 14795.619</f>
-        <v>14795.619000000001</v>
-      </c>
-      <c r="J4" s="11">
-        <f xml:space="preserve"> 14795.619</f>
-        <v>14795.619000000001</v>
+      <c r="B4" s="12">
+        <v>5.7859999999999996</v>
+      </c>
+      <c r="C4" s="12">
+        <v>4.9560000000000004</v>
+      </c>
+      <c r="D4" s="12">
+        <v>11.39361407677</v>
+      </c>
+      <c r="E4" s="16">
+        <v>12571.374</v>
+      </c>
+      <c r="F4" s="16">
+        <v>10890.396000000001</v>
+      </c>
+      <c r="G4" s="16">
+        <v>10908.966</v>
+      </c>
+      <c r="H4" s="16">
+        <v>12589.944</v>
+      </c>
+      <c r="I4" s="16">
+        <v>10890.396000000001</v>
+      </c>
+      <c r="J4" s="16">
+        <v>10908.966</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="8">
-        <v>-5.7350000000000003</v>
-      </c>
-      <c r="C5" s="8">
-        <f>4.951</f>
-        <v>4.9509999999999996</v>
-      </c>
-      <c r="D5" s="15">
-        <v>226700</v>
-      </c>
-      <c r="E5" s="11">
-        <f xml:space="preserve"> 4691596.233</f>
-        <v>4691596.233</v>
-      </c>
-      <c r="F5" s="11">
-        <f>2474084.77</f>
-        <v>2474084.77</v>
-      </c>
-      <c r="G5" s="11">
-        <f>2498581.398</f>
-        <v>2498581.398</v>
-      </c>
-      <c r="H5" s="11">
-        <f>4716092.861</f>
-        <v>4716092.8609999996</v>
-      </c>
-      <c r="I5" s="11">
-        <f>2474084.77</f>
-        <v>2474084.77</v>
-      </c>
-      <c r="J5" s="11">
-        <f>2474084.77</f>
-        <v>2474084.77</v>
+      <c r="B5" s="12">
+        <v>5.5449999999999999</v>
+      </c>
+      <c r="C5" s="12">
+        <v>4.9130000000000003</v>
+      </c>
+      <c r="D5" s="12">
+        <v>226.62857000000002</v>
+      </c>
+      <c r="E5" s="16">
+        <f>3777313.222</f>
+        <v>3777313.2220000001</v>
+      </c>
+      <c r="F5" s="16">
+        <v>2012788.0719999999</v>
+      </c>
+      <c r="G5" s="16">
+        <v>2042312</v>
+      </c>
+      <c r="H5" s="16">
+        <f>797125.945</f>
+        <v>797125.94499999995</v>
+      </c>
+      <c r="I5" s="16">
+        <v>2006921.331</v>
+      </c>
+      <c r="J5" s="16">
+        <f>2028365.838</f>
+        <v>2028365.838</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="8">
-        <v>-6.3390000000000004</v>
-      </c>
-      <c r="C6" s="8">
-        <v>5.0140000000000002</v>
-      </c>
-      <c r="D6" s="15">
-        <v>145250</v>
-      </c>
-      <c r="E6" s="11">
-        <v>3275430.7409999999</v>
-      </c>
-      <c r="F6" s="11">
-        <v>3275430.7409999999</v>
-      </c>
-      <c r="G6" s="11">
-        <f>1742166.519</f>
-        <v>1742166.5190000001</v>
-      </c>
-      <c r="H6" s="11">
-        <v>3292557.7590000001</v>
-      </c>
-      <c r="I6" s="11">
-        <f>1725039.501</f>
-        <v>1725039.5009999999</v>
-      </c>
-      <c r="J6" s="11">
-        <f>1725039.501</f>
-        <v>1725039.5009999999</v>
+      <c r="B6" s="12">
+        <f>6.544</f>
+        <v>6.5439999999999996</v>
+      </c>
+      <c r="C6" s="12">
+        <v>5.0330000000000004</v>
+      </c>
+      <c r="D6" s="12">
+        <v>144.96318500000001</v>
+      </c>
+      <c r="E6" s="16">
+        <f>3173003.125</f>
+        <v>3173003.125</v>
+      </c>
+      <c r="F6" s="16">
+        <v>1673268.895</v>
+      </c>
+      <c r="G6" s="16">
+        <v>1691863.696</v>
+      </c>
+      <c r="H6" s="16">
+        <v>3189510.2740000002</v>
+      </c>
+      <c r="I6" s="16">
+        <v>1674044.84</v>
+      </c>
+      <c r="J6" s="16">
+        <v>1674580.602</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
@@ -789,70 +829,64 @@
         <v>11</v>
       </c>
       <c r="B7" s="8">
-        <v>-6.1390000000000002</v>
+        <v>6.2080000000000002</v>
       </c>
       <c r="C7" s="8">
-        <v>4.9930000000000003</v>
-      </c>
-      <c r="D7" s="15">
-        <v>19503.66</v>
-      </c>
-      <c r="E7" s="11">
-        <f>48263.425</f>
-        <v>48263.425000000003</v>
-      </c>
-      <c r="F7" s="11">
-        <f>34366.627</f>
-        <v>34366.627</v>
-      </c>
-      <c r="G7" s="11">
-        <f>34520.144</f>
-        <v>34520.144</v>
-      </c>
-      <c r="H7" s="11">
-        <f>48416.942</f>
-        <v>48416.942000000003</v>
-      </c>
-      <c r="I7" s="11">
-        <f>34366.627</f>
-        <v>34366.627</v>
-      </c>
-      <c r="J7" s="11">
-        <f xml:space="preserve"> 34366.627</f>
-        <v>34366.627</v>
+        <v>5</v>
+      </c>
+      <c r="D7" s="12">
+        <v>15.734040000000002</v>
+      </c>
+      <c r="E7" s="16">
+        <v>33008.550999999999</v>
+      </c>
+      <c r="F7" s="16">
+        <v>22906.137999999999</v>
+      </c>
+      <c r="G7" s="16">
+        <v>23017.738000000001</v>
+      </c>
+      <c r="H7" s="16">
+        <v>33120.150999999998</v>
+      </c>
+      <c r="I7" s="16">
+        <v>22906.137999999999</v>
+      </c>
+      <c r="J7" s="16">
+        <v>22906.137999999999</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="8">
-        <v>-10.685</v>
-      </c>
-      <c r="C8" s="8">
-        <v>5.4710000000000001</v>
-      </c>
-      <c r="D8" s="15">
-        <v>190000</v>
-      </c>
-      <c r="E8" s="11">
+      <c r="B8" s="12">
+        <v>10.603999999999999</v>
+      </c>
+      <c r="C8" s="12">
+        <v>5.4619999999999997</v>
+      </c>
+      <c r="D8" s="8">
+        <v>190</v>
+      </c>
+      <c r="E8" s="15">
         <f>1382171.187</f>
         <v>1382171.1869999999</v>
       </c>
-      <c r="F8" s="12">
+      <c r="F8" s="16">
         <v>2169261.0989999999</v>
       </c>
-      <c r="G8" s="12">
+      <c r="G8" s="16">
         <v>2160636.7940000002</v>
       </c>
-      <c r="H8" s="12">
+      <c r="H8" s="16">
         <v>1373471.226</v>
       </c>
-      <c r="I8" s="12">
+      <c r="I8" s="16">
         <f>2169281.574</f>
         <v>2169281.574</v>
       </c>
-      <c r="J8" s="12">
+      <c r="J8" s="16">
         <v>2169316.281</v>
       </c>
     </row>
@@ -860,70 +894,71 @@
       <c r="A9" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="8">
-        <v>-0.80900000000000005</v>
-      </c>
-      <c r="C9" s="8">
-        <f>2.705</f>
-        <v>2.7050000000000001</v>
-      </c>
-      <c r="D9" s="15">
-        <v>39433.565000000002</v>
-      </c>
-      <c r="E9" s="11">
-        <f>226119.825</f>
-        <v>226119.82500000001</v>
-      </c>
-      <c r="F9" s="11">
-        <v>291498.44199999998</v>
-      </c>
-      <c r="G9" s="11">
-        <v>303222.84499999997</v>
-      </c>
-      <c r="H9" s="11">
-        <v>483601.223</v>
-      </c>
-      <c r="I9" s="11">
-        <v>595264.56900000002</v>
-      </c>
-      <c r="J9" s="11">
-        <v>370457.00599999999</v>
+      <c r="B9" s="12">
+        <v>0.81200000000000006</v>
+      </c>
+      <c r="C9" s="12">
+        <f>2.697</f>
+        <v>2.6970000000000001</v>
+      </c>
+      <c r="D9" s="8">
+        <v>70.328671184279997</v>
+      </c>
+      <c r="E9" s="16">
+        <f>398972.625</f>
+        <v>398972.625</v>
+      </c>
+      <c r="F9" s="16">
+        <f>515880.092</f>
+        <v>515880.092</v>
+      </c>
+      <c r="G9" s="16">
+        <v>535054.995</v>
+      </c>
+      <c r="H9" s="16">
+        <v>380820.51400000002</v>
+      </c>
+      <c r="I9" s="16">
+        <v>517530.62400000001</v>
+      </c>
+      <c r="J9" s="16">
+        <v>551556.57299999997</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="8">
-        <v>-4.6710000000000003</v>
-      </c>
-      <c r="C10" s="8">
-        <v>4.8390000000000004</v>
-      </c>
-      <c r="D10" s="15">
-        <v>3627.46</v>
-      </c>
-      <c r="E10" s="11">
-        <f>5316.827</f>
-        <v>5316.8270000000002</v>
-      </c>
-      <c r="F10" s="13">
-        <f>2700.551</f>
-        <v>2700.5509999999999</v>
-      </c>
-      <c r="G10" s="11">
-        <v>2729.453</v>
-      </c>
-      <c r="H10" s="11">
-        <v>5345.7290000000003</v>
-      </c>
-      <c r="I10" s="11">
-        <f>2700.551</f>
-        <v>2700.5509999999999</v>
-      </c>
-      <c r="J10" s="11">
-        <f>2700.551</f>
-        <v>2700.5509999999999</v>
+      <c r="B10" s="12">
+        <v>4.593</v>
+      </c>
+      <c r="C10" s="12">
+        <v>4.8310000000000004</v>
+      </c>
+      <c r="D10" s="12">
+        <v>3.94584</v>
+      </c>
+      <c r="E10" s="16">
+        <v>4081.3989999999999</v>
+      </c>
+      <c r="F10" s="16">
+        <f>2064.99</f>
+        <v>2064.9899999999998</v>
+      </c>
+      <c r="G10" s="16">
+        <v>2087.2649999999999</v>
+      </c>
+      <c r="H10" s="16">
+        <f>4103.674</f>
+        <v>4103.674</v>
+      </c>
+      <c r="I10" s="16">
+        <f>2064.99</f>
+        <v>2064.9899999999998</v>
+      </c>
+      <c r="J10" s="16">
+        <f>2064.99</f>
+        <v>2064.9899999999998</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
@@ -936,134 +971,296 @@
       <c r="C11" s="8">
         <v>0.5</v>
       </c>
-      <c r="D11" s="15">
-        <v>50000</v>
-      </c>
-      <c r="E11" s="11">
+      <c r="D11" s="8">
+        <v>50</v>
+      </c>
+      <c r="E11" s="15">
         <v>16666.666000000001</v>
       </c>
-      <c r="F11" s="11">
+      <c r="F11" s="15">
         <v>16666.666000000001</v>
       </c>
-      <c r="G11" s="11">
+      <c r="G11" s="15">
         <v>25000</v>
       </c>
-      <c r="H11" s="11">
+      <c r="H11" s="15">
         <v>16757.718000000001</v>
       </c>
-      <c r="I11" s="11">
+      <c r="I11" s="15">
         <v>17017.325000000001</v>
       </c>
-      <c r="J11" s="11">
+      <c r="J11" s="15">
         <v>24558.29</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B12" s="9">
-        <v>-5.3559999999999999</v>
-      </c>
-      <c r="C12" s="9">
-        <v>4.9109999999999996</v>
-      </c>
-      <c r="D12" s="16">
-        <v>4699</v>
-      </c>
-      <c r="E12" s="11">
-        <f>8083.881</f>
-        <v>8083.8810000000003</v>
-      </c>
-      <c r="F12" s="11">
-        <v>4104.4449999999997</v>
-      </c>
-      <c r="G12" s="14">
-        <v>4148.4059999999999</v>
-      </c>
-      <c r="H12" s="11">
-        <v>8127.8410000000003</v>
-      </c>
-      <c r="I12" s="11">
-        <f>4104.445</f>
-        <v>4104.4449999999997</v>
-      </c>
-      <c r="J12" s="11">
-        <f>4104.445</f>
-        <v>4104.4449999999997</v>
+        <v>30</v>
+      </c>
+      <c r="B12" s="12">
+        <f>6.582</f>
+        <v>6.5819999999999999</v>
+      </c>
+      <c r="C12" s="12">
+        <v>5.04</v>
+      </c>
+      <c r="D12" s="12">
+        <v>2.23</v>
+      </c>
+      <c r="E12" s="16">
+        <f>3515.423</f>
+        <v>3515.4229999999998</v>
+      </c>
+      <c r="F12" s="15">
+        <v>1784</v>
+      </c>
+      <c r="G12" s="16">
+        <v>1803.127</v>
+      </c>
+      <c r="H12" s="16">
+        <v>3534.55</v>
+      </c>
+      <c r="I12" s="15">
+        <v>1784</v>
+      </c>
+      <c r="J12" s="15">
+        <v>1784</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B13" s="8">
-        <v>-6.9480000000000004</v>
-      </c>
-      <c r="C13" s="8">
-        <v>5.0780000000000003</v>
-      </c>
-      <c r="D13" s="16">
-        <v>4699</v>
-      </c>
-      <c r="E13" s="11">
-        <f>8083.882</f>
-        <v>8083.8819999999996</v>
-      </c>
-      <c r="F13" s="11">
-        <v>4104.4449999999997</v>
-      </c>
-      <c r="G13" s="14">
-        <v>4148.4059999999999</v>
-      </c>
-      <c r="H13" s="11">
-        <v>8127.8410000000003</v>
-      </c>
-      <c r="I13" s="11">
-        <f>4104.445</f>
-        <v>4104.4449999999997</v>
-      </c>
-      <c r="J13" s="11">
-        <f>4104.445</f>
-        <v>4104.4449999999997</v>
+        <v>31</v>
+      </c>
+      <c r="B13" s="12">
+        <f>5.388</f>
+        <v>5.3879999999999999</v>
+      </c>
+      <c r="C13" s="12">
+        <v>4.9139999999999997</v>
+      </c>
+      <c r="D13" s="12">
+        <v>5.6639999999999997</v>
+      </c>
+      <c r="E13" s="16">
+        <v>8929.5349999999999</v>
+      </c>
+      <c r="F13" s="16">
+        <f>4592.985</f>
+        <v>4592.9849999999997</v>
+      </c>
+      <c r="G13" s="16">
+        <v>4640.8900000000003</v>
+      </c>
+      <c r="H13" s="16">
+        <f>8977.44</f>
+        <v>8977.44</v>
+      </c>
+      <c r="I13" s="16">
+        <f>4592.985</f>
+        <v>4592.9849999999997</v>
+      </c>
+      <c r="J13" s="16">
+        <f>4592.985</f>
+        <v>4592.9849999999997</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="10">
-        <v>-5.718</v>
-      </c>
-      <c r="C14" s="10">
-        <v>4.048</v>
-      </c>
-      <c r="D14" s="17">
-        <v>797275.03899999999</v>
-      </c>
-      <c r="E14" s="12">
-        <v>13442265.551999999</v>
-      </c>
-      <c r="F14" s="12">
-        <v>21116729.438999999</v>
-      </c>
-      <c r="G14" s="12">
-        <v>18382414.385000002</v>
-      </c>
-      <c r="H14" s="12">
-        <v>12476517.574999999</v>
-      </c>
-      <c r="I14" s="12">
-        <f>21041508.831</f>
-        <v>21041508.831</v>
-      </c>
-      <c r="J14" s="12">
-        <v>19423382.971000001</v>
-      </c>
+      <c r="B14" s="12">
+        <v>5.4859999999999998</v>
+      </c>
+      <c r="C14" s="12">
+        <v>3.9780000000000002</v>
+      </c>
+      <c r="D14" s="18">
+        <v>820.88792026104989</v>
+      </c>
+      <c r="E14" s="16">
+        <v>12607277.468</v>
+      </c>
+      <c r="F14" s="16">
+        <v>21433958.388999999</v>
+      </c>
+      <c r="G14" s="16">
+        <v>18682468.258000001</v>
+      </c>
+      <c r="H14" s="16">
+        <v>11603661.220000001</v>
+      </c>
+      <c r="I14" s="16">
+        <v>21352830.381999999</v>
+      </c>
+      <c r="J14" s="16">
+        <v>19767212.513</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" s="14">
+        <v>3.9449999999999998</v>
+      </c>
+      <c r="C15" s="14">
+        <v>3.3519999999999999</v>
+      </c>
+      <c r="D15" s="12">
+        <v>630.88800000000003</v>
+      </c>
+      <c r="E15" s="16">
+        <v>10680747</v>
+      </c>
+      <c r="F15" s="16">
+        <v>122447810</v>
+      </c>
+      <c r="G15" s="17">
+        <v>10046187</v>
+      </c>
+      <c r="H15" s="17">
+        <v>10011379</v>
+      </c>
+      <c r="I15" s="17">
+        <v>12173784</v>
+      </c>
+      <c r="J15" s="17">
+        <v>10786480</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="D16" s="13"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42DE1351-9820-4849-99B5-2D788A7FDE9C}">
+  <dimension ref="A1:D12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2">
+        <f xml:space="preserve"> 7.939773/2</f>
+        <v>3.9698864999999999</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="9">
+        <v>11.272</v>
+      </c>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5">
+        <f>B4-B2*TAN(B3*PI()/180)</f>
+        <v>10.994398493277419</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7">
+        <f>B5</f>
+        <v>10.994398493277419</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8">
+        <f>B7*COS(6*PI()/180)</f>
+        <v>10.934170027968348</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="11"/>
+      <c r="B10" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" s="11">
+        <v>11.026999999999999</v>
+      </c>
+      <c r="C11" s="10">
+        <v>226631</v>
+      </c>
+      <c r="D11" s="11">
+        <f>C11/B11</f>
+        <v>20552.371451890816</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" s="11">
+        <v>15.7</v>
+      </c>
+      <c r="C12" s="10">
+        <v>144962</v>
+      </c>
+      <c r="D12" s="11">
+        <f>C12/B12</f>
+        <v>9233.248407643312</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
 </file>
</xml_diff>